<commit_message>
Load by query params, fixed rowspan bug
</commit_message>
<xml_diff>
--- a/TestPWA/wwwroot/checklist/CIS.xlsx
+++ b/TestPWA/wwwroot/checklist/CIS.xlsx
@@ -814,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
@@ -878,6 +878,9 @@
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="7" applyBorder="1" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="3" applyFill="1" borderId="9" applyBorder="1" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="13" applyBorder="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1202,32 +1205,32 @@
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
       <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
     </row>
     <row r="19">
       <c r="A19" s="22" t="s">

</xml_diff>